<commit_message>
Fuentes de los Webservices
</commit_message>
<xml_diff>
--- a/URLS People.xlsx
+++ b/URLS People.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>Accion</t>
   </si>
@@ -41,54 +41,30 @@
     <t>http://localhost:8080/WebSkillsGW7/webresources/entis.people/</t>
   </si>
   <si>
-    <t>http://localhost:8080/WebSkillsGW7/webresources/entis.people/login</t>
-  </si>
-  <si>
-    <t>{"email":"Lorena.Portillo@Garonz.com","pasword":"MD5"}</t>
-  </si>
-  <si>
-    <t>{"idpeople":1,"name":"Lorena","lastname":"Portillo","email":"Lorena.Portillo@Garonz.com","indate":1481515200000,"pasword":"MD5","jobtitle":"Licenciada","fotolink":"link","foto":null,"ischangepassword":"T","idrol":{"idrol":1,"name":"SuperAdmin"}}</t>
-  </si>
-  <si>
     <t>POST</t>
   </si>
   <si>
     <t>People CREATE</t>
   </si>
   <si>
-    <t>{"name":"Andres","lastname":"Gonzalez","email":"Andres.Gonzalez@Garonz.com","indate":1481515200000,"pasword":"MD5","jobtitle":"Licenciado","fotolink":"link","foto":null,"ischangepassword":"T","idrol":3}</t>
-  </si>
-  <si>
     <t>PUT</t>
   </si>
   <si>
-    <t>{"idpeople":1,"name":"Jose","lastname":"Gonzalez","email":"Andres@Garonz.com","indate":1481515200000,"pasword":"MD5","jobtitle":"Licenciado","fotolink":"link","foto":null,"ischangepassword":"T","idrol":3}</t>
-  </si>
-  <si>
     <t>{"idpeople":1}</t>
   </si>
   <si>
-    <t>http://localhost:8080/WebSkillsGW7/webresources/entis.people/find</t>
-  </si>
-  <si>
     <t>DELETE</t>
   </si>
   <si>
     <t>{"idpeople":3}</t>
   </si>
   <si>
-    <t>[{"idpeople":2,"name":"Laura","lastname":"Perez","email":"Laura.Perez@Garonz.com","indate":1478836800000,"pasword":"MD5","jobtitle":"Ingeniero","fotolink":"link","foto":null,"ischangepassword":"F","idrol":{"idrol":2,"name":"Admin"}},{"idpeople":3,"name":"Andres","lastname":"Gonzalez","email":"Andres.@Garonz.Gonzalezcom","indate":1481515200000,"pasword":"MD5","jobtitle":"Licenciado","fotolink":"link","foto":null,"ischangepassword":"T","idrol":{"idrol":3,"name":"Watcher"}},{"idpeople":1,"name":"Jose","lastname":"Gonzalez","email":"Andres@Garonz.com","indate":1481515200000,"pasword":"MD5","jobtitle":"Licenciado","fotolink":"link","foto":null,"ischangepassword":"T","idrol":{"idrol":3,"name":"Watcher"}}]</t>
-  </si>
-  <si>
     <t>GET</t>
   </si>
   <si>
     <t>http://localhost:8080/WebSkillsGW7/webresources/entis.people/1/2</t>
   </si>
   <si>
-    <t>[{"idpeople":3,"name":"Andres","lastname":"Gonzalez","email":"Andres.@Garonz.Gonzalezcom","indate":1481515200000,"pasword":"MD5","jobtitle":"Licenciado","fotolink":"link","foto":null,"ischangepassword":"T","idrol":{"idrol":3,"name":"Watcher"}},{"idpeople":1,"name":"Jose","lastname":"Gonzalez","email":"Andres@Garonz.com","indate":1481515200000,"pasword":"MD5","jobtitle":"Licenciado","fotolink":"link","foto":null,"ischangepassword":"T","idrol":{"idrol":3,"name":"Watcher"}}]</t>
-  </si>
-  <si>
     <t>http://localhost:8080/WebSkillsGW7/webresources/entis.people/count</t>
   </si>
   <si>
@@ -111,6 +87,191 @@
   </si>
   <si>
     <t>LOGIN</t>
+  </si>
+  <si>
+    <t>[
+      {
+      "idpeople": 2,
+      "name": "Laura",
+      "lastname": "Perez",
+      "email": "Laura.Perez@Garonz.com",
+      "phone": "Laura.Perez@Garonz.com",
+      "location": null,
+      "indate": 1478836800000,
+      "pasword": "MD5MD5",
+      "jobtitle": "Ingeniero",
+      "fotolink": "link",
+      "foto": null,
+      "ischangepassword": "F",
+      "idrol":       {
+         "idrol": 2,
+         "name": "Admin"
+      }
+   },
+      {
+      "idpeople": 3,
+      "name": "Andres",
+      "lastname": "Gonzalez",
+      "email": "AndresGonzales@Garonz.com",
+      "phone": "AndresGonzales@Garonz.com",
+      "location": null,
+      "indate": 1481515200000,
+      "pasword": "MD5MD5",
+      "jobtitle": "Licenciado",
+      "fotolink": "link",
+      "foto": null,
+      "ischangepassword": "T",
+      "idrol":       {
+         "idrol": 3,
+         "name": "Watcher"
+      }
+   }
+]</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/WebSkillsGW7/webresources/entis.people/find/</t>
+  </si>
+  <si>
+    <t>{
+   "name": "Jose",
+   "lastname": "Gonzalez",
+   "email": "Andres@Garonz.com",
+   "phone": null,
+   "location": null,
+   "indate": 1481515200000,
+   "pasword": "MD5MD5",
+   "jobtitle": "Licenciado",
+   "fotolink": "link",
+   "foto": null,
+   "ischangepassword": "T",
+   "idrol":    {
+      "idrol": 3,
+      "name": "Watcher"
+   }
+}</t>
+  </si>
+  <si>
+    <t>{  "idpeople": 1,
+   "name": "Jose",
+   "lastname": "Gonzalez",
+   "email": "Andres@Garonz.com",
+   "phone": null,
+   "location": null,
+   "indate": 1481515200000,
+   "pasword": "MD5MD5",
+   "jobtitle": "Licenciado",
+   "fotolink": "link",
+   "foto": null,
+   "ischangepassword": "T",
+   "idrol":    {
+      "idrol": 3,
+      "name": "Watcher"
+   }
+}</t>
+  </si>
+  <si>
+    <t>{
+   "idpeople": 1,
+   "name": "Jose",
+   "lastname": "Gonzalez",
+   "email": "Andres@Garonz.com",
+   "phone": null,
+   "location": null,
+   "indate": 1481515200000,
+   "pasword": "MD5MD5",
+   "jobtitle": "Licenciado",
+   "fotolink": "link",
+   "foto": null,
+   "ischangepassword": "T",
+   "idrol":    {
+      "idrol": 3,
+      "name": "Watcher"
+   }
+}</t>
+  </si>
+  <si>
+    <t>[
+      {
+      "idpeople": 1,
+      "name": "Jose",
+      "lastname": "Gonzalez",
+      "email": "Andres@Garonz.com",
+      "phone": null,
+      "location": null,
+      "indate": 1481515200000,
+      "pasword": "MD5MD5",
+      "jobtitle": "Licenciado",
+      "fotolink": "link",
+      "foto": null,
+      "ischangepassword": "T",
+      "idrol":       {
+         "idrol": 3,
+         "name": "Watcher"
+      }
+   },
+      {
+      "idpeople": 2,
+      "name": "Laura",
+      "lastname": "Perez",
+      "email": "Laura.Perez@Garonz.com",
+      "phone": null,
+      "location": null,
+      "indate": 1478836800000,
+      "pasword": "MD5MD5",
+      "jobtitle": "Ingeniero",
+      "fotolink": "link",
+      "foto": null,
+      "ischangepassword": "F",
+      "idrol":       {
+         "idrol": 2,
+         "name": "Admin"
+      }
+   },
+      {
+      "idpeople": 3,
+      "name": "Andres",
+      "lastname": "Gonzalez",
+      "email": "AndresGonzales@Garonz.com",
+      "phone":  null,
+      "location": null,
+      "indate": 1481515200000,
+      "pasword": "MD5MD5",
+      "jobtitle": "Licenciado",
+      "fotolink": "link",
+      "foto": null,
+      "ischangepassword": "T",
+      "idrol":       {
+         "idrol": 3,
+         "name": "Watcher"
+      }
+   }
+]</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/WebSkillsGW7/webresources/entis.people/login/</t>
+  </si>
+  <si>
+    <t>{
+   "idpeople": 2,
+   "name": "Laura",
+   "lastname": "Perez",
+   "email": "Laura.Perez@Garonz.com",
+   "phone": null,
+   "location": null,
+   "indate": 1478836800000,
+   "pasword": "MD5MD5",
+   "jobtitle": "Ingeniero",
+   "fotolink": "link",
+   "foto": null,
+   "ischangepassword": "F",
+   "idrol":    {
+      "idrol": 2,
+      "name": "Admin"
+   }
+}</t>
+  </si>
+  <si>
+    <t>{"email":"Laura.Perez@Garonz.com","pasword":"MD5MD5"}</t>
   </si>
 </sst>
 </file>
@@ -478,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,117 +667,117 @@
     </row>
     <row r="3" spans="1:5" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="255" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="255" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="270" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="240" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E18">
         <v>3</v>

</xml_diff>